<commit_message>
Them dong bo du lieu voi GA Them confirm khi delete
</commit_message>
<xml_diff>
--- a/Documents/báo cáo tủ giày.xlsx
+++ b/Documents/báo cáo tủ giày.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminlocal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\18.HOANHT\Phan-Mem-Cua-Cong-Ty\C#\LOCKER\UMCLocker\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$79</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="8">
   <si>
     <t>Từ tủ</t>
   </si>
@@ -365,13 +368,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68:D79"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="109.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1045,7 +1051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>108</v>
       </c>
@@ -1059,7 +1065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>269</v>
       </c>
@@ -1073,7 +1079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>250</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>56</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>111</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>271</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>207</v>
       </c>
@@ -1143,7 +1149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7</v>
       </c>
@@ -1171,7 +1177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>14</v>
       </c>
@@ -1185,7 +1191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>24</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>13</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>35</v>
       </c>
@@ -1226,8 +1232,22 @@
       <c r="D61" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="str">
+        <f>CONCATENATE("insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(",F61,",162,'AVAIABLE','F')")</f>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(2,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F61">
+        <v>2</v>
+      </c>
+      <c r="P61">
+        <v>2</v>
+      </c>
+      <c r="Q61">
+        <f>P61+P62</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>41</v>
       </c>
@@ -1240,8 +1260,18 @@
       <c r="D62" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="str">
+        <f t="shared" ref="E62:E71" si="0">CONCATENATE("insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(",F62,",162,'AVAIABLE','F')")</f>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(3,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F62">
+        <v>3</v>
+      </c>
+      <c r="P62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>40</v>
       </c>
@@ -1254,8 +1284,18 @@
       <c r="D63" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(4,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F63">
+        <v>4</v>
+      </c>
+      <c r="P63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>49</v>
       </c>
@@ -1268,8 +1308,18 @@
       <c r="D64" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(5,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F64">
+        <v>5</v>
+      </c>
+      <c r="P64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>100</v>
       </c>
@@ -1282,8 +1332,18 @@
       <c r="D65" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(6,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F65">
+        <v>6</v>
+      </c>
+      <c r="P65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>12</v>
       </c>
@@ -1296,8 +1356,18 @@
       <c r="D66" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(7,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F66">
+        <v>7</v>
+      </c>
+      <c r="P66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>52</v>
       </c>
@@ -1310,8 +1380,18 @@
       <c r="D67" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(8,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F67">
+        <v>8</v>
+      </c>
+      <c r="P67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1</v>
       </c>
@@ -1324,8 +1404,18 @@
       <c r="D68" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(11,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F68">
+        <v>11</v>
+      </c>
+      <c r="P68">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>17</v>
       </c>
@@ -1338,8 +1428,18 @@
       <c r="D69" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(12,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F69">
+        <v>12</v>
+      </c>
+      <c r="P69">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>15</v>
       </c>
@@ -1352,8 +1452,15 @@
       <c r="D70" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(1,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>19</v>
       </c>
@@ -1366,8 +1473,15 @@
       <c r="D71" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into [UMCLOCKER].[dbo].[Locker](locker_index, locker_number,state,locker_type) values(9,162,'AVAIABLE','F')</v>
+      </c>
+      <c r="F71">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>21</v>
       </c>
@@ -1381,7 +1495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>29</v>
       </c>
@@ -1395,7 +1509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>28</v>
       </c>
@@ -1409,7 +1523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>30</v>
       </c>
@@ -1423,7 +1537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>35</v>
       </c>
@@ -1437,7 +1551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>99</v>
       </c>
@@ -1451,7 +1565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>98</v>
       </c>
@@ -1465,7 +1579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>102</v>
       </c>
@@ -1479,7 +1593,36 @@
         <v>6</v>
       </c>
     </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>162</v>
+      </c>
+      <c r="B80">
+        <v>162</v>
+      </c>
+      <c r="C80">
+        <v>12</v>
+      </c>
+      <c r="D80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>165</v>
+      </c>
+      <c r="B81">
+        <v>165</v>
+      </c>
+      <c r="C81">
+        <v>12</v>
+      </c>
+      <c r="D81" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:A79"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sửa lỗi phần đồng bộ hóa
</commit_message>
<xml_diff>
--- a/Documents/báo cáo tủ giày.xlsx
+++ b/Documents/báo cáo tủ giày.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$1:$D$85</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="8">
   <si>
     <t>Từ tủ</t>
   </si>
@@ -368,10 +368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q81"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61:E71"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -407,7 +408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>127</v>
       </c>
@@ -421,7 +422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>132</v>
       </c>
@@ -435,7 +436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>139</v>
       </c>
@@ -449,7 +450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>156</v>
       </c>
@@ -463,7 +464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>163</v>
       </c>
@@ -477,7 +478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>166</v>
       </c>
@@ -491,7 +492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>128</v>
       </c>
@@ -505,7 +506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>138</v>
       </c>
@@ -519,7 +520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>230</v>
       </c>
@@ -533,7 +534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>243</v>
       </c>
@@ -547,7 +548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>259</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>7</v>
       </c>
@@ -1177,7 +1178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>14</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>24</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>13</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>35</v>
       </c>
@@ -1247,7 +1248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>41</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>40</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>49</v>
       </c>
@@ -1319,7 +1320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>100</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>12</v>
       </c>
@@ -1367,7 +1368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>52</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1</v>
       </c>
@@ -1415,7 +1416,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>17</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>15</v>
       </c>
@@ -1460,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>19</v>
       </c>
@@ -1481,7 +1482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>21</v>
       </c>
@@ -1495,7 +1496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>29</v>
       </c>
@@ -1509,7 +1510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>28</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>30</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>35</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>99</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>98</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>102</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>162</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>165</v>
       </c>
@@ -1621,8 +1622,70 @@
         <v>4</v>
       </c>
     </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>21</v>
+      </c>
+      <c r="B82">
+        <v>21</v>
+      </c>
+      <c r="C82">
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>37</v>
+      </c>
+      <c r="B83">
+        <v>37</v>
+      </c>
+      <c r="C83">
+        <v>9</v>
+      </c>
+      <c r="D83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>20</v>
+      </c>
+      <c r="B84">
+        <v>20</v>
+      </c>
+      <c r="C84">
+        <v>9</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>14</v>
+      </c>
+      <c r="B85">
+        <v>14</v>
+      </c>
+      <c r="C85">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A79"/>
+  <autoFilter ref="D1:D85">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Locker nam"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>